<commit_message>
updated divisions and NL
</commit_message>
<xml_diff>
--- a/NL/MEX.xlsx
+++ b/NL/MEX.xlsx
@@ -93013,13 +93013,13 @@
         <v>1594</v>
       </c>
       <c r="C11" t="s">
-        <v>857</v>
+        <v>1002</v>
       </c>
       <c r="D11" t="s">
-        <v>1156</v>
+        <v>739</v>
       </c>
       <c r="E11" t="s">
-        <v>1108</v>
+        <v>965</v>
       </c>
     </row>
   </sheetData>
@@ -93181,10 +93181,10 @@
         <v>1594</v>
       </c>
       <c r="C11" t="s">
-        <v>1212</v>
+        <v>1309</v>
       </c>
       <c r="D11" t="s">
-        <v>749</v>
+        <v>918</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated new leagues divs
</commit_message>
<xml_diff>
--- a/NL/MEX.xlsx
+++ b/NL/MEX.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11908" uniqueCount="1614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11917" uniqueCount="1615">
   <si>
     <t>Atl..San.Luis</t>
   </si>
@@ -4861,6 +4861,9 @@
   </si>
   <si>
     <t>2021/2022</t>
+  </si>
+  <si>
+    <t>2022/2023</t>
   </si>
   <si>
     <t>N</t>
@@ -93465,6 +93468,23 @@
         <v>1091</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1612</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D12" t="s">
+        <v>820</v>
+      </c>
+      <c r="E12" t="s">
+        <v>751</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -93484,10 +93504,10 @@
         <v>1600</v>
       </c>
       <c r="C1" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="D1" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="2">
@@ -93628,6 +93648,20 @@
       </c>
       <c r="D11" t="s">
         <v>1144</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1612</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>